<commit_message>
updated and working need to check the data
</commit_message>
<xml_diff>
--- a/Sizing/motorData/M13-M34 performance curve 20200916.xlsx
+++ b/Sizing/motorData/M13-M34 performance curve 20200916.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CEE6B8-C5E3-4086-BDF5-E64EA27824D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E07FE09-0930-477C-A881-0E853A47B14C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-345" yWindow="690" windowWidth="24060" windowHeight="19320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -100,8 +100,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -160,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,6 +190,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,1284 +668,11 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>M13C9_48VDC</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Peak Torque </c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$7:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>31.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15.75</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>14</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0B59-4088-AB2F-86B9D376D82D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Continuous Torque</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$7:$E$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.571428571428573</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.5000000000000009</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.6666666666666679</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0B59-4088-AB2F-86B9D376D82D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="233935232"/>
-        <c:axId val="233937152"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Peak Power</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$D$7:$D$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.8324607329842932</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.6649214659685865</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6.5968586387434556</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0B59-4088-AB2F-86B9D376D82D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Continuous Power</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$7:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$F$7:$F$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.62827225130890052</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.256544502617801</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.261780104712042</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5130890052356021</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1413612565445028</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3.1413612565445028</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.1413612565445028</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1413612565445028</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.1413612565445028</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0B59-4088-AB2F-86B9D376D82D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="233945344"/>
-        <c:axId val="233943424"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="233935232"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Speed [rpm]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233937152"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="233937152"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Torque</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> [Nm]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233935232"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="233943424"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Power [KW]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233945344"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="233945344"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233943424"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>M15C6_48VDC</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Peak Torque</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$7:$H$16</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2650</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$I$7:$I$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43.773584905660378</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>38.666666666666664</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>33.142857142857146</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>25.777777777777779</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B8D4-4AC3-AC37-554CB5DDF579}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Continuous Torque</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$7:$H$16</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2650</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$K$7:$K$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>15.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.628571428571428</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11.925000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10.6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B8D4-4AC3-AC37-554CB5DDF579}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="233981824"/>
-        <c:axId val="233992192"/>
-      </c:scatterChart>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Peak Power</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$7:$H$16</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2650</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$J$7:$J$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0366492146596857</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0732984293193715</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.1099476439790568</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12.146596858638743</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B8D4-4AC3-AC37-554CB5DDF579}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Continuous Power</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:prstDash val="sysDash"/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$H$7:$H$16</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2650</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3500</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4500</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$L$7:$L$16</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.94240837696335078</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.8848167539267016</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.8272251308900525</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7696335078534031</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.994764397905759</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.994764397905759</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.994764397905759</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4.994764397905759</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.994764397905759</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B8D4-4AC3-AC37-554CB5DDF579}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="234004480"/>
-        <c:axId val="233994112"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="233981824"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Speed</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> [rpm]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233992192"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="233992192"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Torque [Nm]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233981824"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="233994112"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Power</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> [KW]</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="234004480"/>
-        <c:crosses val="max"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="234004480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233994112"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="lt1"/>
-    </a:solidFill>
-    <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1"/>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr>
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:latin typeface="+mn-lt"/>
-          <a:ea typeface="+mn-ea"/>
-          <a:cs typeface="+mn-cs"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="171" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1952,7 +683,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8658311" cy="6281351"/>
+    <xdr:ext cx="8661623" cy="6277588"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1978,85 +709,6 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>90486</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>742949</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>781049</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2383,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:BM62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X37" sqref="X37"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA11" sqref="BA11:BA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2806,7 +1458,7 @@
       <c r="AS7" s="2">
         <v>0</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AT7" s="14">
         <f>AR7/AP7</f>
         <v>0.37068965517241381</v>
       </c>
@@ -2825,7 +1477,7 @@
       <c r="AZ7" s="2">
         <v>0</v>
       </c>
-      <c r="BA7" s="2">
+      <c r="BA7" s="14">
         <f>AY7/AW7</f>
         <v>0.39946140035906641</v>
       </c>
@@ -2978,7 +1630,7 @@
       <c r="AS8" s="2">
         <v>11.256544502617801</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AT8" s="14">
         <f t="shared" ref="AT8:AT22" si="3">AR8/AP8</f>
         <v>0.37068965517241381</v>
       </c>
@@ -2997,7 +1649,7 @@
       <c r="AZ8" s="2">
         <v>23.298429319371728</v>
       </c>
-      <c r="BA8" s="2">
+      <c r="BA8" s="14">
         <f t="shared" ref="BA8:BA16" si="4">AY8/AW8</f>
         <v>0.39946140035906641</v>
       </c>
@@ -3150,7 +1802,7 @@
       <c r="AS9" s="2">
         <v>22.513089005235603</v>
       </c>
-      <c r="AT9" s="2">
+      <c r="AT9" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -3169,7 +1821,7 @@
       <c r="AZ9" s="2">
         <v>46.596858638743456</v>
       </c>
-      <c r="BA9" s="2">
+      <c r="BA9" s="14">
         <f t="shared" si="4"/>
         <v>0.39946140035906641</v>
       </c>
@@ -3322,7 +1974,7 @@
       <c r="AS10" s="2">
         <v>33.769633507853406</v>
       </c>
-      <c r="AT10" s="2">
+      <c r="AT10" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -3341,7 +1993,7 @@
       <c r="AZ10" s="2">
         <v>72.691099476439788</v>
       </c>
-      <c r="BA10" s="2">
+      <c r="BA10" s="14">
         <f t="shared" si="4"/>
         <v>0.39946140035906641</v>
       </c>
@@ -3494,7 +2146,7 @@
       <c r="AS11" s="2">
         <v>45.026178010471206</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AT11" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -3513,7 +2165,7 @@
       <c r="AZ11" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA11" s="2">
+      <c r="BA11" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003682</v>
       </c>
@@ -3666,7 +2318,7 @@
       <c r="AS12" s="2">
         <v>56.282722513089006</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AT12" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -3685,7 +2337,7 @@
       <c r="AZ12" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA12" s="2">
+      <c r="BA12" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003682</v>
       </c>
@@ -3838,7 +2490,7 @@
       <c r="AS13" s="2">
         <v>67.539267015706812</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -3857,7 +2509,7 @@
       <c r="AZ13" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA13" s="2">
+      <c r="BA13" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003687</v>
       </c>
@@ -4010,7 +2662,7 @@
       <c r="AS14" s="2">
         <v>80.821989528795811</v>
       </c>
-      <c r="AT14" s="2">
+      <c r="AT14" s="14">
         <f t="shared" si="3"/>
         <v>0.37068965517241381</v>
       </c>
@@ -4029,7 +2681,7 @@
       <c r="AZ14" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA14" s="2">
+      <c r="BA14" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003682</v>
       </c>
@@ -4182,7 +2834,7 @@
       <c r="AS15" s="2">
         <v>90.052356020942412</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AT15" s="14">
         <f t="shared" si="3"/>
         <v>0.41302468542887333</v>
       </c>
@@ -4201,7 +2853,7 @@
       <c r="AZ15" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA15" s="2">
+      <c r="BA15" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003682</v>
       </c>
@@ -4354,7 +3006,7 @@
       <c r="AS16" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AT16" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853614</v>
       </c>
@@ -4373,7 +3025,7 @@
       <c r="AZ16" s="2">
         <v>80.985340314136124</v>
       </c>
-      <c r="BA16" s="2">
+      <c r="BA16" s="14">
         <f t="shared" si="4"/>
         <v>0.44504097040003676</v>
       </c>
@@ -4496,7 +3148,7 @@
       <c r="AS17" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT17" s="2">
+      <c r="AT17" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853619</v>
       </c>
@@ -4619,7 +3271,7 @@
       <c r="AS18" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT18" s="2">
+      <c r="AT18" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853619</v>
       </c>
@@ -4742,7 +3394,7 @@
       <c r="AS19" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT19" s="2">
+      <c r="AT19" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853619</v>
       </c>
@@ -4850,7 +3502,7 @@
       <c r="AS20" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT20" s="2">
+      <c r="AT20" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853608</v>
       </c>
@@ -4958,7 +3610,7 @@
       <c r="AS21" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT21" s="2">
+      <c r="AT21" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853614</v>
       </c>
@@ -5066,7 +3718,7 @@
       <c r="AS22" s="2">
         <v>96.018324607329845</v>
       </c>
-      <c r="AT22" s="2">
+      <c r="AT22" s="14">
         <f t="shared" si="3"/>
         <v>0.44038757083853619</v>
       </c>
@@ -5909,7 +4561,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5944,6 +4595,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAE60540A1AE0C40A57867F6D1668AAB" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a077bfdb5c83a9e90026d9660a1fda64">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f0b06742-ce3d-43d6-80c6-a38c29477f3b" xmlns:ns3="ac8b36ea-85bd-4ee9-9a25-ec081feb3b1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ab75e0c3651772810f3079df645c8c4c" ns2:_="" ns3:_="">
     <xsd:import namespace="f0b06742-ce3d-43d6-80c6-a38c29477f3b"/>
@@ -6148,15 +4808,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C887559-7771-4403-8D1D-96BB517FF6B2}">
   <ds:schemaRefs>
@@ -6167,6 +4818,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F39AACE-8895-4AA7-A7CC-069EC4C6B0D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADADBB7C-17F4-4F6F-BBC4-57C2C59FD103}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6183,12 +4842,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F39AACE-8895-4AA7-A7CC-069EC4C6B0D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>